<commit_message>
.do/requestmapping의 관계, index.jsp/board.jsp, jsp포워드
</commit_message>
<xml_diff>
--- a/스프링자습서.xlsx
+++ b/스프링자습서.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\spring\workspace\springboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74D6AA38-C00B-4EA5-89E2-E314C8782093}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45DA7AD3-ECF8-4393-8EBD-5AE2AEE605BD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12390" yWindow="2280" windowWidth="23265" windowHeight="9300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12390" yWindow="2280" windowWidth="23265" windowHeight="9300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>1.JDK란?</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -186,6 +186,13 @@
   <si>
     <t>3.InteliJ</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>환경변수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://mongodev.tistory.com/28</t>
   </si>
 </sst>
 </file>
@@ -531,7 +538,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:H17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
@@ -625,10 +632,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{638C221B-4C07-4A37-A927-1FAA68557331}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -651,11 +658,23 @@
         <v>12</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B7" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" xr:uid="{57950C1D-8AB6-48A3-B052-2AB1A6244AE7}"/>
+    <hyperlink ref="B7" r:id="rId2" xr:uid="{BF42E10E-1FB6-4B03-97EA-DA51048A9830}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>